<commit_message>
se demora mucho seguimos mejorando
</commit_message>
<xml_diff>
--- a/Schuman List.xlsx
+++ b/Schuman List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\X1\Documents\Schuman\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B62C3E7-F533-4A60-AABC-18FD031B6E78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02EC6D6C-7F43-44A0-A4BA-17AA0E64030A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{1D924867-5138-4414-9B39-ADB0E20E2123}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>Site</t>
   </si>
@@ -144,7 +144,7 @@
     <t>C:\Users\X1\Documents\Schuman\WORD files\RITM0483421_Angoi Ludovic Nguessan NGORAN.docx</t>
   </si>
   <si>
-    <t>FAILED: Call was rejected by callee. (Exception from HRESULT: 0x80010001 (RPC_E_CALL_REJECTED))</t>
+    <t>C:\Users\X1\Documents\Schuman\WORD files\RITM0483421_Angoi Ludovic Nguessan NGORAN.pdf</t>
   </si>
 </sst>
 </file>
@@ -4620,10 +4620,13 @@
         <v>22</v>
       </c>
       <c r="G3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H3" t="s">
         <v>34</v>
+      </c>
+      <c r="I3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
dashboard a filter working
</commit_message>
<xml_diff>
--- a/Schuman List.xlsx
+++ b/Schuman List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\X1\Documents\Schuman\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D7F4BA-3EDB-4E0E-917D-AFFA7E8B1922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51AC63A7-AEC9-42B7-A555-3831FC943144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{2FE17FE1-ABF7-4DC1-A8B0-257EE915A712}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Agent</t>
   </si>
@@ -71,88 +71,16 @@
     <t>PI History / Comment</t>
   </si>
   <si>
-    <t>RITM0493918</t>
-  </si>
-  <si>
-    <t>RITM0493919</t>
-  </si>
-  <si>
-    <t>RITM0493920</t>
-  </si>
-  <si>
-    <t>RITM0427680</t>
-  </si>
-  <si>
-    <t>RITM0105308</t>
-  </si>
-  <si>
-    <t>RITM0104655</t>
-  </si>
-  <si>
-    <t>INC0404926</t>
-  </si>
-  <si>
-    <t>Sara AHMAD TORRES</t>
-  </si>
-  <si>
-    <t>Complete</t>
-  </si>
-  <si>
-    <t>No open tasks.</t>
-  </si>
-  <si>
-    <t>Ledio AHMETAJ</t>
-  </si>
-  <si>
-    <t>Antoine Patrick Colin ANDRAULT</t>
-  </si>
-  <si>
-    <t>Juan DIOSES</t>
-  </si>
-  <si>
-    <t>MUSTBRUN2424012</t>
-  </si>
-  <si>
-    <t>CEBOLLA NICUESA Mireia</t>
-  </si>
-  <si>
-    <t>02PI20200923448</t>
-  </si>
-  <si>
-    <t>Zeljana VUKOVIĆ</t>
-  </si>
-  <si>
-    <t>PRESBRUN1907058</t>
-  </si>
-  <si>
-    <t>Juan Emilio AYUSO GONZÁLEZ</t>
-  </si>
-  <si>
-    <t>02PI20242016586</t>
-  </si>
-  <si>
-    <t>OK</t>
-  </si>
-  <si>
-    <t>C:\Users\X1\Documents\Schuman\WORD files\RITM0493918_Sara AHMAD TORRES.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\X1\Documents\Schuman\WORD files\RITM0493919_Ledio AHMETAJ.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\X1\Documents\Schuman\WORD files\RITM0493920_Antoine Patrick Colin ANDRAULT.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\X1\Documents\Schuman\WORD files\RITM0427680_Juan DIOSES.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\X1\Documents\Schuman\WORD files\RITM0105308_CEBOLLA NICUESA Mireia.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\X1\Documents\Schuman\WORD files\RITM0104655_Zeljana VUKOVIĆ.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\X1\Documents\Schuman\WORD files\INC0404926_Juan Emilio AYUSO GONZÁLEZ.pdf</t>
+    <t>RITM0496748</t>
+  </si>
+  <si>
+    <t>Dashboard Status</t>
+  </si>
+  <si>
+    <t>Present Time</t>
+  </si>
+  <si>
+    <t>Closed Time</t>
   </si>
 </sst>
 </file>
@@ -541,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D15FE3B-AD84-45CF-9592-EB018CC38643}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -556,7 +484,7 @@
     <col min="6" max="6" width="14.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -590,165 +518,24 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D2" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" t="s">
-        <v>31</v>
-      </c>
-      <c r="J2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" t="s">
-        <v>31</v>
-      </c>
-      <c r="J5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" t="s">
-        <v>31</v>
-      </c>
-      <c r="J6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" t="s">
-        <v>31</v>
-      </c>
-      <c r="J7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" t="s">
-        <v>31</v>
-      </c>
-      <c r="J8" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{FAA87AE1-4395-49C6-A11D-99301DD89BDE}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{1B31E10D-4F05-42E2-9A65-7461A7910912}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{7D0CB081-C59C-4B9D-AD50-95BD132BEC86}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{2EE54EBB-BC4C-4E8A-9392-BF9B1AAF7288}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{0CDE91AA-1C72-442C-A026-9B30753B94B9}"/>
-    <hyperlink ref="D7" r:id="rId6" xr:uid="{66A7C67C-44F1-4809-8C48-2B65F0D3C131}"/>
-    <hyperlink ref="D8" r:id="rId7" xr:uid="{3691564E-4A69-4035-BC4E-E7A114EB3442}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{4A55F518-BC43-4F4B-A736-71A3525F9099}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
working check-in and -out
</commit_message>
<xml_diff>
--- a/Schuman List.xlsx
+++ b/Schuman List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\X1\Documents\Schuman\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72FC698C-A0C2-488E-B750-6320000C6E90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451FCF65-A745-43C4-ADF0-8FE100A00E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{2FE17FE1-ABF7-4DC1-A8B0-257EE915A712}"/>
   </bookViews>
@@ -98,7 +98,7 @@
     <t>PARENT</t>
   </si>
   <si>
-    <t>Appointment</t>
+    <t>Checked-In</t>
   </si>
 </sst>
 </file>
@@ -578,8 +578,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{662D740C-96B0-4ABE-9484-C8ED08851606}"/>
-    <hyperlink ref="F2" r:id="rId2" xr:uid="{CBA8F583-0467-46BA-B344-E2A847E46AF1}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{73311D4D-641F-45A6-93BB-91B9312B0485}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{B495E860-4463-4AF1-B828-0F80D6783D19}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
hacinedo cambios ya que cuando hay mas de 10 se demora mucho
</commit_message>
<xml_diff>
--- a/Schuman List.xlsx
+++ b/Schuman List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\X1\Documents\Schuman\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D909EE-A88D-406B-AFF9-D11A3084D328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4359E22E-24F7-4920-9FAB-B11A7B505D52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{2FE17FE1-ABF7-4DC1-A8B0-257EE915A712}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="225">
   <si>
     <t>Agent</t>
   </si>
@@ -92,6 +92,213 @@
     <t>RITM0493120</t>
   </si>
   <si>
+    <t>INC0404030</t>
+  </si>
+  <si>
+    <t>INC0405320</t>
+  </si>
+  <si>
+    <t>INC0404913</t>
+  </si>
+  <si>
+    <t>INC0404662</t>
+  </si>
+  <si>
+    <t>INC0403929</t>
+  </si>
+  <si>
+    <t>INC0404073</t>
+  </si>
+  <si>
+    <t>INC0398334</t>
+  </si>
+  <si>
+    <t>INC0400192</t>
+  </si>
+  <si>
+    <t>INC0399952</t>
+  </si>
+  <si>
+    <t>INC0399909</t>
+  </si>
+  <si>
+    <t>INC0399906</t>
+  </si>
+  <si>
+    <t>INC0398797</t>
+  </si>
+  <si>
+    <t>INC0399068</t>
+  </si>
+  <si>
+    <t>INC0398566</t>
+  </si>
+  <si>
+    <t>INC0397938</t>
+  </si>
+  <si>
+    <t>INC0396829</t>
+  </si>
+  <si>
+    <t>INC0390677</t>
+  </si>
+  <si>
+    <t>INC0384484</t>
+  </si>
+  <si>
+    <t>INC0396867</t>
+  </si>
+  <si>
+    <t>INC0393533</t>
+  </si>
+  <si>
+    <t>INC0393530</t>
+  </si>
+  <si>
+    <t>INC0393057</t>
+  </si>
+  <si>
+    <t>INC0392998</t>
+  </si>
+  <si>
+    <t>INC0386947</t>
+  </si>
+  <si>
+    <t>INC0381429</t>
+  </si>
+  <si>
+    <t>INC0381995</t>
+  </si>
+  <si>
+    <t>INC0377661</t>
+  </si>
+  <si>
+    <t>INC0376136</t>
+  </si>
+  <si>
+    <t>INC0377128</t>
+  </si>
+  <si>
+    <t>INC0376121</t>
+  </si>
+  <si>
+    <t>INC0375309</t>
+  </si>
+  <si>
+    <t>INC0372528</t>
+  </si>
+  <si>
+    <t>INC0373224</t>
+  </si>
+  <si>
+    <t>INC0374026</t>
+  </si>
+  <si>
+    <t>INC0370735</t>
+  </si>
+  <si>
+    <t>INC0365085</t>
+  </si>
+  <si>
+    <t>INC0368029</t>
+  </si>
+  <si>
+    <t>INC0370558</t>
+  </si>
+  <si>
+    <t>INC0372344</t>
+  </si>
+  <si>
+    <t>INC0353533</t>
+  </si>
+  <si>
+    <t>INC0367376</t>
+  </si>
+  <si>
+    <t>INC0350488</t>
+  </si>
+  <si>
+    <t>INC0346775</t>
+  </si>
+  <si>
+    <t>INC0370773</t>
+  </si>
+  <si>
+    <t>INC0370852</t>
+  </si>
+  <si>
+    <t>INC0370721</t>
+  </si>
+  <si>
+    <t>INC0357741</t>
+  </si>
+  <si>
+    <t>INC0240792</t>
+  </si>
+  <si>
+    <t>INC0357389</t>
+  </si>
+  <si>
+    <t>INC0354452</t>
+  </si>
+  <si>
+    <t>RITM0395760</t>
+  </si>
+  <si>
+    <t>RITM0400363</t>
+  </si>
+  <si>
+    <t>RITM0400334</t>
+  </si>
+  <si>
+    <t>RITM0429435</t>
+  </si>
+  <si>
+    <t>RITM0430321</t>
+  </si>
+  <si>
+    <t>RITM0430778</t>
+  </si>
+  <si>
+    <t>RITM0400091</t>
+  </si>
+  <si>
+    <t>RITM0400088</t>
+  </si>
+  <si>
+    <t>RITM0420978</t>
+  </si>
+  <si>
+    <t>RITM0405042</t>
+  </si>
+  <si>
+    <t>RITM0433027</t>
+  </si>
+  <si>
+    <t>RITM0433109</t>
+  </si>
+  <si>
+    <t>RITM0433132</t>
+  </si>
+  <si>
+    <t>RITM0433154</t>
+  </si>
+  <si>
+    <t>RITM0433331</t>
+  </si>
+  <si>
+    <t>RITM0420972</t>
+  </si>
+  <si>
+    <t>RITM0434588</t>
+  </si>
+  <si>
+    <t>RITM0434592</t>
+  </si>
+  <si>
+    <t>RITM0434593</t>
+  </si>
+  <si>
     <t>Juan Carlos DIOSES</t>
   </si>
   <si>
@@ -119,38 +326,398 @@
     <t>SCTASK0880081</t>
   </si>
   <si>
-    <t>AUTO</t>
-  </si>
-  <si>
-    <t>SCTASK0762732</t>
-  </si>
-  <si>
-    <t>SCTASK0784120</t>
-  </si>
-  <si>
-    <t>SCTASK0784119</t>
-  </si>
-  <si>
-    <t>OK</t>
-  </si>
-  <si>
-    <t>C:\Users\X1\Documents\Schuman\WORD files\2026-02-17\20260217 - RITM0496748 - DIOSES-JUAN-CARLOS.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\X1\Documents\Schuman\WORD files\2026-02-17\20260217 - RITM0405052 - TORNACO-ALEXANDRA-DE.pdf</t>
-  </si>
-  <si>
-    <t>SKIPPED: PDF exists</t>
-  </si>
-  <si>
-    <t>C:\Users\X1\Documents\Schuman\WORD files\2026-02-17\20260217 - RITM0493120 - KORZENIECKA-ANETA.pdf</t>
+    <t>Natalia Maria VALENCIA AGUIRRE</t>
+  </si>
+  <si>
+    <t>MUSTBRUN2425371</t>
+  </si>
+  <si>
+    <t>Georgiana SANDU</t>
+  </si>
+  <si>
+    <t>MUSTBRUN2334714</t>
+  </si>
+  <si>
+    <t>Klaudia ARBETOVA</t>
+  </si>
+  <si>
+    <t>MUSTBRUN2421355</t>
+  </si>
+  <si>
+    <t>Gabriel Stanislav Vladimir LITERA</t>
+  </si>
+  <si>
+    <t>Sandrina MARCUZZO</t>
+  </si>
+  <si>
+    <t>MUSTBRUN2425125</t>
+  </si>
+  <si>
+    <t>Marika SULANKO</t>
+  </si>
+  <si>
+    <t>MUSTBRUN2420461</t>
+  </si>
+  <si>
+    <t>Anastasia COUCOURATOS</t>
+  </si>
+  <si>
+    <t>02PI20140917135</t>
+  </si>
+  <si>
+    <t>Liselotte JENSEN</t>
+  </si>
+  <si>
+    <t>Lucie Agnès Marie Olga MAISTRELLI</t>
+  </si>
+  <si>
+    <t>Kristýna MAŤÁTKOVÁ</t>
+  </si>
+  <si>
+    <t>Ana RADOČAJ</t>
+  </si>
+  <si>
+    <t>Angelika KISS</t>
+  </si>
+  <si>
+    <t>MUSTBRUN2420747</t>
+  </si>
+  <si>
+    <t>Maria Nazareth ECHART ORUS</t>
+  </si>
+  <si>
+    <t>MUSTBRUN2333965</t>
+  </si>
+  <si>
+    <t>Krista DANKERE</t>
+  </si>
+  <si>
+    <t>MUSTBRUN2036708</t>
+  </si>
+  <si>
+    <t>Maja SABOL</t>
+  </si>
+  <si>
+    <t>Cristina SANCHEZ VILLA</t>
+  </si>
+  <si>
+    <t>02PI20233264742, MUSTBRUN2423446</t>
+  </si>
+  <si>
+    <t>Wojciech KUZMA</t>
+  </si>
+  <si>
+    <t>Tajana LJUBIČIĆ</t>
+  </si>
+  <si>
+    <t>MUSTBRUN2334472</t>
+  </si>
+  <si>
+    <t>Luc JEUNESSE</t>
+  </si>
+  <si>
+    <t>02PI20242843962</t>
+  </si>
+  <si>
+    <t>Maria Antoaneta NEAG</t>
+  </si>
+  <si>
+    <t>02PI20242705674</t>
+  </si>
+  <si>
+    <t>Kateřina HEROUTOVÁ</t>
+  </si>
+  <si>
+    <t>MUSTBRUN2420940</t>
+  </si>
+  <si>
+    <t>Igor DEQUECKER</t>
+  </si>
+  <si>
+    <t>02PI20191989578, 02PI2019198578</t>
+  </si>
+  <si>
+    <t>Christos PAPAGIANNIS</t>
+  </si>
+  <si>
+    <t>02PI20242397849</t>
+  </si>
+  <si>
+    <t>Nicolas DORGERET</t>
+  </si>
+  <si>
+    <t>MUSTBRUN2508215</t>
+  </si>
+  <si>
+    <t>Ramune TAMASAUSKAITE</t>
+  </si>
+  <si>
+    <t>02PI20242016283, 02PI20233397147</t>
+  </si>
+  <si>
+    <t>Cesar Augusto CASTELLO MORENO</t>
+  </si>
+  <si>
+    <t>MUSTBRUN2426375</t>
+  </si>
+  <si>
+    <t>Alina Leandra Ó RIADA</t>
+  </si>
+  <si>
+    <t>02PI20203679120</t>
+  </si>
+  <si>
+    <t>02PI20242136678</t>
+  </si>
+  <si>
+    <t>Francesco BARCHIELLI</t>
+  </si>
+  <si>
+    <t>02PI20242360243WASI</t>
+  </si>
+  <si>
+    <t>Anna ARESU</t>
+  </si>
+  <si>
+    <t>MUSTBRUN2425910</t>
+  </si>
+  <si>
+    <t>Stephanie HONNEFELDER</t>
+  </si>
+  <si>
+    <t>MUSTBRUN2508216</t>
+  </si>
+  <si>
+    <t>Philine SCHOLZE</t>
+  </si>
+  <si>
+    <t>MUSTBRUN2421735, 02PI20250819606</t>
+  </si>
+  <si>
+    <t>Ariane DEBYSER</t>
+  </si>
+  <si>
+    <t>MUSTBRUN2425050</t>
+  </si>
+  <si>
+    <t>Rachid AHAJJAM</t>
+  </si>
+  <si>
+    <t>MUSTBRUN2421304</t>
+  </si>
+  <si>
+    <t>Gianna GRIGÒ</t>
+  </si>
+  <si>
+    <t>MUSTBRUN2421392</t>
+  </si>
+  <si>
+    <t>Fabiola VALENTINI</t>
+  </si>
+  <si>
+    <t>MUSTBRUN2423870</t>
+  </si>
+  <si>
+    <t>Maria TOADER</t>
+  </si>
+  <si>
+    <t>02PI20241996977</t>
+  </si>
+  <si>
+    <t>Samuel DE LEMOS PEIXOTO</t>
+  </si>
+  <si>
+    <t>02PI20231287180</t>
+  </si>
+  <si>
+    <t>Elise HANCOTTE</t>
+  </si>
+  <si>
+    <t>Ellen Sarah VAN NIEUWENHUYZE</t>
+  </si>
+  <si>
+    <t>MUSTBRUN2421379</t>
+  </si>
+  <si>
+    <t>Anastasia MITRONATSIOU</t>
+  </si>
+  <si>
+    <t>MUSTBRUN2425798</t>
+  </si>
+  <si>
+    <t>5c7518931beb241018d65398624bcb08</t>
+  </si>
+  <si>
+    <t>MUSTBRUN2425955</t>
+  </si>
+  <si>
+    <t>David SCHWANDER</t>
+  </si>
+  <si>
+    <t>MUSTBRUN2425390</t>
+  </si>
+  <si>
+    <t>Karin SAUERTEIG</t>
+  </si>
+  <si>
+    <t>02PI20200227608</t>
+  </si>
+  <si>
+    <t>Barbara KRAFT</t>
+  </si>
+  <si>
+    <t>MUSTBRUN2332364</t>
+  </si>
+  <si>
+    <t>Virginie REMACLE</t>
+  </si>
+  <si>
+    <t>MUSTBRUN2426486</t>
+  </si>
+  <si>
+    <t>Ana SÁEZ-BENITO CAUVILLA</t>
+  </si>
+  <si>
+    <t>Bettina BLASIG</t>
+  </si>
+  <si>
+    <t>02PI20210751648</t>
+  </si>
+  <si>
+    <t>Cedric Franz K GOOR</t>
+  </si>
+  <si>
+    <t>MUSTBRUN2115651</t>
+  </si>
+  <si>
+    <t>Maria-teresa GONZALEZ CABALLERO</t>
+  </si>
+  <si>
+    <t>Tania DE POORTER</t>
+  </si>
+  <si>
+    <t>MUSTBRUN2421299</t>
+  </si>
+  <si>
+    <t>SCTASK0689026</t>
+  </si>
+  <si>
+    <t>Dora Cristina BARREIRA RAMOS</t>
+  </si>
+  <si>
+    <t>MUSTBRUN2420933</t>
+  </si>
+  <si>
+    <t>SCTASK0698388</t>
+  </si>
+  <si>
+    <t>Devrim ATES</t>
+  </si>
+  <si>
+    <t>MUSTBRUN2425474</t>
+  </si>
+  <si>
+    <t>SCTASK0698363</t>
+  </si>
+  <si>
+    <t>SCTASK0756216</t>
+  </si>
+  <si>
+    <t>SCTASK0758095</t>
+  </si>
+  <si>
+    <t>Satu Simona POUTANEN</t>
+  </si>
+  <si>
+    <t>SCTASK0758952</t>
+  </si>
+  <si>
+    <t>Lina BARSTYTE</t>
+  </si>
+  <si>
+    <t>MUSTBRUN2424523</t>
+  </si>
+  <si>
+    <t>SCTASK0698111</t>
+  </si>
+  <si>
+    <t>Johannes LITZELMANN</t>
+  </si>
+  <si>
+    <t>MUSTBRUN2424524</t>
+  </si>
+  <si>
+    <t>SCTASK0698108</t>
+  </si>
+  <si>
+    <t>Michael Alexander SPEISER</t>
+  </si>
+  <si>
+    <t>MUSTBRUN2505542</t>
+  </si>
+  <si>
+    <t>SCTASK0739497</t>
+  </si>
+  <si>
+    <t>Susan NITSCHE</t>
+  </si>
+  <si>
+    <t>SCTASK0708526</t>
+  </si>
+  <si>
+    <t>Giulia PASCUZZI</t>
+  </si>
+  <si>
+    <t>SCTASK0763066</t>
+  </si>
+  <si>
+    <t>Léa Lucie Léontine SAUBION</t>
+  </si>
+  <si>
+    <t>SCTASK0763194</t>
+  </si>
+  <si>
+    <t>Noémie Kerfalie Helena Jane-Nolwe NGANGA</t>
+  </si>
+  <si>
+    <t>SCTASK0763230</t>
+  </si>
+  <si>
+    <t>SCTASK0763271</t>
+  </si>
+  <si>
+    <t>Jauram REISNER</t>
+  </si>
+  <si>
+    <t>SCTASK0763566</t>
+  </si>
+  <si>
+    <t>Laura PROIETTI</t>
+  </si>
+  <si>
+    <t>MUSTBRUN2423960</t>
+  </si>
+  <si>
+    <t>SCTASK0739491</t>
+  </si>
+  <si>
+    <t>New EP User</t>
+  </si>
+  <si>
+    <t>SCTASK0765919</t>
+  </si>
+  <si>
+    <t>SCTASK0765928</t>
+  </si>
+  <si>
+    <t>SCTASK0765931</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,6 +734,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -189,18 +763,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{1D7AC411-0A0C-4C5D-BF15-F6D769099F62}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -532,10 +1111,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D15FE3B-AD84-45CF-9592-EB018CC38643}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:O2"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D306" sqref="D81:D306"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -596,168 +1175,1313 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>18</v>
+        <v>87</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>88</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" t="s">
-        <v>31</v>
-      </c>
-      <c r="J2" t="s">
-        <v>32</v>
+        <v>89</v>
       </c>
       <c r="O2" t="s">
-        <v>21</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>22</v>
+        <v>91</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>92</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>88</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" t="s">
-        <v>33</v>
+        <v>93</v>
       </c>
       <c r="O3" t="s">
-        <v>21</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>88</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" t="s">
-        <v>34</v>
-      </c>
-      <c r="J4" t="s">
-        <v>33</v>
+        <v>95</v>
       </c>
       <c r="O4" t="s">
-        <v>27</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>22</v>
+        <v>96</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>16</v>
+        <v>97</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" t="s">
-        <v>34</v>
-      </c>
-      <c r="J5" t="s">
-        <v>33</v>
-      </c>
-      <c r="O5" t="s">
-        <v>27</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>22</v>
+        <v>98</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>16</v>
+        <v>99</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6" t="s">
-        <v>33</v>
-      </c>
-      <c r="O6" t="s">
-        <v>27</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" t="s">
+        <v>108</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>109</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="2" t="s">
+      <c r="E12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H7" t="s">
+      <c r="E13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>112</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" t="s">
+        <v>114</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C17" t="s">
+        <v>116</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>117</v>
+      </c>
+      <c r="C18" t="s">
+        <v>118</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J7" t="s">
+      <c r="E18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>119</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>120</v>
+      </c>
+      <c r="C20" t="s">
+        <v>121</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>122</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>123</v>
+      </c>
+      <c r="C22" t="s">
+        <v>124</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="O7" t="s">
-        <v>21</v>
+      <c r="E22" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>125</v>
+      </c>
+      <c r="C23" t="s">
+        <v>126</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>127</v>
+      </c>
+      <c r="C24" t="s">
+        <v>128</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>129</v>
+      </c>
+      <c r="C25" t="s">
+        <v>130</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>131</v>
+      </c>
+      <c r="C26" t="s">
+        <v>132</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>133</v>
+      </c>
+      <c r="C27" t="s">
+        <v>134</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>135</v>
+      </c>
+      <c r="C28" t="s">
+        <v>136</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E28" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>137</v>
+      </c>
+      <c r="C29" t="s">
+        <v>138</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B30" t="s">
+        <v>139</v>
+      </c>
+      <c r="C30" t="s">
+        <v>140</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
+        <v>141</v>
+      </c>
+      <c r="C31" t="s">
+        <v>142</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
+        <v>131</v>
+      </c>
+      <c r="C32" t="s">
+        <v>143</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E32" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B33" t="s">
+        <v>144</v>
+      </c>
+      <c r="C33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
+        <v>146</v>
+      </c>
+      <c r="C34" t="s">
+        <v>147</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E34" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
+        <v>148</v>
+      </c>
+      <c r="C35" t="s">
+        <v>149</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E35" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
+        <v>150</v>
+      </c>
+      <c r="C36" t="s">
+        <v>151</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E36" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>152</v>
+      </c>
+      <c r="C37" t="s">
+        <v>153</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E37" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B38" t="s">
+        <v>154</v>
+      </c>
+      <c r="C38" t="s">
+        <v>155</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E38" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B39" t="s">
+        <v>156</v>
+      </c>
+      <c r="C39" t="s">
+        <v>157</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E39" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B40" t="s">
+        <v>158</v>
+      </c>
+      <c r="C40" t="s">
+        <v>159</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E40" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B41" t="s">
+        <v>160</v>
+      </c>
+      <c r="C41" t="s">
+        <v>161</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E41" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B42" t="s">
+        <v>162</v>
+      </c>
+      <c r="C42" t="s">
+        <v>163</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E42" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B43" t="s">
+        <v>164</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E43" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B44" t="s">
+        <v>165</v>
+      </c>
+      <c r="C44" t="s">
+        <v>166</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E44" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B45" t="s">
+        <v>167</v>
+      </c>
+      <c r="C45" t="s">
+        <v>168</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E45" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B46" t="s">
+        <v>169</v>
+      </c>
+      <c r="C46" t="s">
+        <v>170</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E46" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B47" t="s">
+        <v>171</v>
+      </c>
+      <c r="C47" t="s">
+        <v>172</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E47" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B48" t="s">
+        <v>173</v>
+      </c>
+      <c r="C48" t="s">
+        <v>174</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E48" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="49" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B49" t="s">
+        <v>175</v>
+      </c>
+      <c r="C49" t="s">
+        <v>176</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E49" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="50" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B50" t="s">
+        <v>177</v>
+      </c>
+      <c r="C50" t="s">
+        <v>178</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E50" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="51" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B51" t="s">
+        <v>179</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E51" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="52" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B52" t="s">
+        <v>180</v>
+      </c>
+      <c r="C52" t="s">
+        <v>181</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E52" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="53" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B53" t="s">
+        <v>182</v>
+      </c>
+      <c r="C53" t="s">
+        <v>183</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E53" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="54" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B54" t="s">
+        <v>184</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E54" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="55" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B55" t="s">
+        <v>185</v>
+      </c>
+      <c r="C55" t="s">
+        <v>186</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E55" t="s">
+        <v>88</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="O55" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="56" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B56" t="s">
+        <v>185</v>
+      </c>
+      <c r="C56" t="s">
+        <v>186</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E56" t="s">
+        <v>88</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="O56" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="57" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B57" t="s">
+        <v>188</v>
+      </c>
+      <c r="C57" t="s">
+        <v>189</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E57" t="s">
+        <v>88</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="O57" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="58" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B58" t="s">
+        <v>188</v>
+      </c>
+      <c r="C58" t="s">
+        <v>189</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E58" t="s">
+        <v>88</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="O58" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="59" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B59" t="s">
+        <v>191</v>
+      </c>
+      <c r="C59" t="s">
+        <v>192</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E59" t="s">
+        <v>88</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="O59" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="60" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B60" t="s">
+        <v>191</v>
+      </c>
+      <c r="C60" t="s">
+        <v>192</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E60" t="s">
+        <v>88</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="O60" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="61" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B61" t="s">
+        <v>87</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E61" t="s">
+        <v>88</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="O61" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="62" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B62" t="s">
+        <v>87</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E62" t="s">
+        <v>88</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="O62" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="63" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B63" t="s">
+        <v>87</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E63" t="s">
+        <v>88</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="O63" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="64" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B64" t="s">
+        <v>196</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E64" t="s">
+        <v>88</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="O64" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="65" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B65" t="s">
+        <v>198</v>
+      </c>
+      <c r="C65" t="s">
+        <v>199</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E65" t="s">
+        <v>88</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="O65" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="66" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B66" t="s">
+        <v>201</v>
+      </c>
+      <c r="C66" t="s">
+        <v>202</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E66" t="s">
+        <v>88</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="O66" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="67" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B67" t="s">
+        <v>204</v>
+      </c>
+      <c r="C67" t="s">
+        <v>205</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E67" t="s">
+        <v>88</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="O67" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="68" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B68" t="s">
+        <v>207</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E68" t="s">
+        <v>88</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="O68" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="69" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B69" t="s">
+        <v>209</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E69" t="s">
+        <v>88</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="O69" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="70" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B70" t="s">
+        <v>211</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E70" t="s">
+        <v>88</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="O70" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="71" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B71" t="s">
+        <v>213</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E71" t="s">
+        <v>88</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="O71" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="72" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B72" t="s">
+        <v>87</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E72" t="s">
+        <v>88</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="O72" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="73" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B73" t="s">
+        <v>216</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E73" t="s">
+        <v>88</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="O73" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="74" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B74" t="s">
+        <v>218</v>
+      </c>
+      <c r="C74" t="s">
+        <v>219</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E74" t="s">
+        <v>88</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="O74" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="75" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B75" t="s">
+        <v>218</v>
+      </c>
+      <c r="C75" t="s">
+        <v>219</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E75" t="s">
+        <v>88</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="O75" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="76" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B76" t="s">
+        <v>221</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E76" t="s">
+        <v>88</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="O76" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="77" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B77" t="s">
+        <v>221</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E77" t="s">
+        <v>88</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="O77" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="78" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B78" t="s">
+        <v>221</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E78" t="s">
+        <v>88</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="O78" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="79" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B79" t="s">
+        <v>221</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E79" t="s">
+        <v>88</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="O79" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="80" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B80" t="s">
+        <v>221</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E80" t="s">
+        <v>88</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="O80" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{6BDCF609-DA45-40F0-800B-D767797CC244}"/>
-    <hyperlink ref="F2" r:id="rId2" xr:uid="{A3950CE5-653D-4AF7-B185-CF4171C067C0}"/>
-    <hyperlink ref="D3" r:id="rId3" xr:uid="{7491E02F-0EBB-4210-96F8-B9DD8F501625}"/>
-    <hyperlink ref="F3" r:id="rId4" xr:uid="{BED1028C-CC3F-44F7-9110-85FAA2349DE0}"/>
-    <hyperlink ref="D7" r:id="rId5" xr:uid="{DFD6A39F-6312-486F-9B92-E4D617B5D9AE}"/>
-    <hyperlink ref="F7" r:id="rId6" xr:uid="{2C5D0CB5-9DC6-4D7F-A053-A102B8AA1D31}"/>
-    <hyperlink ref="D4" r:id="rId7" xr:uid="{AC1E3E0F-F27B-43C5-A99A-070624E83B82}"/>
-    <hyperlink ref="F4" r:id="rId8" xr:uid="{C345EA21-D8AB-4C68-BFF4-6EA0ADFA6C3E}"/>
-    <hyperlink ref="D5" r:id="rId9" xr:uid="{1983DA36-5D5D-461A-81A2-04F7416D6F10}"/>
-    <hyperlink ref="F5" r:id="rId10" xr:uid="{46B83890-D148-4794-B0B5-18387F83FAEB}"/>
-    <hyperlink ref="D6" r:id="rId11" xr:uid="{C5457092-D105-4FB7-B337-4B532C49F2BF}"/>
-    <hyperlink ref="F6" r:id="rId12" xr:uid="{788A258A-316A-43CD-9A61-5D87F94BE399}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{BA17A53B-7B69-4A8F-B5D5-943D15D604FE}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{C3CC3A3B-4E52-4294-A92F-1AD1CF131189}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{9990B10D-1867-43D9-BA0D-47C428B6CBCD}"/>
+    <hyperlink ref="F3" r:id="rId4" xr:uid="{4D8C5D9A-14DE-4C57-9E19-C63645210BFD}"/>
+    <hyperlink ref="D4" r:id="rId5" xr:uid="{9631E2DE-DB49-4F6E-948F-A2CDDD22AF4F}"/>
+    <hyperlink ref="F4" r:id="rId6" xr:uid="{54B28011-56EF-456F-9D3F-A31BEB6393E2}"/>
+    <hyperlink ref="D5" r:id="rId7" xr:uid="{AE85A689-8A92-4ABE-B668-1CD1CFE4DBC0}"/>
+    <hyperlink ref="D6" r:id="rId8" xr:uid="{66D0B9DF-21ED-4003-83D2-3CD285F8D6C8}"/>
+    <hyperlink ref="D7" r:id="rId9" xr:uid="{EF59744B-870F-4AB0-BB1F-8FCB0A9DEFF5}"/>
+    <hyperlink ref="D8" r:id="rId10" xr:uid="{8DEF0158-A4E1-4D25-ADC4-92F2547DFC3F}"/>
+    <hyperlink ref="D9" r:id="rId11" xr:uid="{8AF21DE4-95AE-49BF-B02A-CC7567716124}"/>
+    <hyperlink ref="D10" r:id="rId12" xr:uid="{2480E105-0B71-4AA5-B50A-265F3102622C}"/>
+    <hyperlink ref="D11" r:id="rId13" xr:uid="{72A9A5E0-B280-44A7-988D-E51DDD075C35}"/>
+    <hyperlink ref="D12" r:id="rId14" xr:uid="{4C3CF96B-6412-4390-9C4A-2314221BC426}"/>
+    <hyperlink ref="D13" r:id="rId15" xr:uid="{EB42D5F1-5681-47B8-B34D-C04DD89513FC}"/>
+    <hyperlink ref="D14" r:id="rId16" xr:uid="{76CD3254-22A3-4D1D-9642-6E6ED376DF4C}"/>
+    <hyperlink ref="D15" r:id="rId17" xr:uid="{270D2E4F-E509-4916-9474-C04D07DACD1C}"/>
+    <hyperlink ref="D16" r:id="rId18" xr:uid="{895634BA-2CC8-4695-BA28-32A488BEB08D}"/>
+    <hyperlink ref="D17" r:id="rId19" xr:uid="{C84836E6-0154-4145-9A24-54D519674506}"/>
+    <hyperlink ref="D18" r:id="rId20" xr:uid="{9EE9D938-AD8E-4A5C-AF12-31247581DDE5}"/>
+    <hyperlink ref="D19" r:id="rId21" xr:uid="{324D88AC-6211-4BD3-AAAA-2FED0E0C0DDF}"/>
+    <hyperlink ref="D20" r:id="rId22" xr:uid="{538A9B9D-6AD6-4340-8E4D-C41EC0EA70F3}"/>
+    <hyperlink ref="D21" r:id="rId23" xr:uid="{7DAD3274-3725-4B55-A2EE-FD313CA1EF96}"/>
+    <hyperlink ref="D22" r:id="rId24" xr:uid="{5A999CE5-FDBE-446D-AFE8-5CEC90C76CB2}"/>
+    <hyperlink ref="D23" r:id="rId25" xr:uid="{512B40F0-87B8-4759-9EA4-1C93F251A2F2}"/>
+    <hyperlink ref="D24" r:id="rId26" xr:uid="{C0F0B46E-470A-4160-9596-8D58C6E05629}"/>
+    <hyperlink ref="D25" r:id="rId27" xr:uid="{78778294-8E95-426A-ABA3-4200C666D0DC}"/>
+    <hyperlink ref="D26" r:id="rId28" xr:uid="{6AE6A030-F62A-43F7-A658-B6B5F123D159}"/>
+    <hyperlink ref="D27" r:id="rId29" xr:uid="{42B0C14A-2CB0-4B08-B197-C3C20C4CED37}"/>
+    <hyperlink ref="D28" r:id="rId30" xr:uid="{932751A1-0CA0-43D7-AC66-158524D3DBD5}"/>
+    <hyperlink ref="D29" r:id="rId31" xr:uid="{9D3F7916-CEFE-4225-B1DF-C61F2521BBE5}"/>
+    <hyperlink ref="D30" r:id="rId32" xr:uid="{DF590D16-8B2F-4637-9C73-5C49F205AF18}"/>
+    <hyperlink ref="D31" r:id="rId33" xr:uid="{64102501-E7D2-4043-8E59-30848F4F59CD}"/>
+    <hyperlink ref="D32" r:id="rId34" xr:uid="{0971E17C-2513-4629-8756-0EB1A1EC4F56}"/>
+    <hyperlink ref="D33" r:id="rId35" xr:uid="{DACDF5E9-DAC2-41DA-87A8-4CA83A5182B6}"/>
+    <hyperlink ref="D34" r:id="rId36" xr:uid="{85CB0FDD-8E9E-44E6-898A-E9EBFA593177}"/>
+    <hyperlink ref="D35" r:id="rId37" xr:uid="{D8E53470-01E7-4182-87C1-3C466D565240}"/>
+    <hyperlink ref="D36" r:id="rId38" xr:uid="{85A5BE0C-C8C5-41ED-8AC8-5010C7666D39}"/>
+    <hyperlink ref="D37" r:id="rId39" xr:uid="{29F89F9A-0B1B-4DB0-B240-9E14D7B8C360}"/>
+    <hyperlink ref="D38" r:id="rId40" xr:uid="{0A85C1AB-F5FB-4111-A7C0-D0D508C57F1B}"/>
+    <hyperlink ref="D39" r:id="rId41" xr:uid="{44486809-320E-479B-BBD8-F7E7A968CC6C}"/>
+    <hyperlink ref="D40" r:id="rId42" xr:uid="{DE68AF30-1D52-4D5A-9ACA-2A67CE737FD4}"/>
+    <hyperlink ref="D41" r:id="rId43" xr:uid="{B813B7C1-0FA6-4A68-96D8-94B201E3E28E}"/>
+    <hyperlink ref="D42" r:id="rId44" xr:uid="{1DA0B7B3-29EC-49B3-84B4-8C253C1E60F0}"/>
+    <hyperlink ref="D43" r:id="rId45" xr:uid="{571625F1-9CBD-4D34-9E9C-3CBE6131AA5A}"/>
+    <hyperlink ref="D44" r:id="rId46" xr:uid="{DB25D749-3424-4B22-9C0A-A85DAD33A870}"/>
+    <hyperlink ref="D45" r:id="rId47" xr:uid="{DCE77E6C-0159-4054-9178-469CE87DDB3B}"/>
+    <hyperlink ref="D46" r:id="rId48" xr:uid="{F01E9A25-2EA8-418B-B161-AD050013D801}"/>
+    <hyperlink ref="D47" r:id="rId49" xr:uid="{A9C50FDD-634A-461A-8695-67293685B98B}"/>
+    <hyperlink ref="D48" r:id="rId50" xr:uid="{7901BD5B-5088-466A-B9D2-2090454524E6}"/>
+    <hyperlink ref="D49" r:id="rId51" xr:uid="{16B6A56B-0C89-4B6B-BA0B-19BAB304EB64}"/>
+    <hyperlink ref="D50" r:id="rId52" xr:uid="{A8D26A38-5DFF-4A6C-B391-8F6489A3B139}"/>
+    <hyperlink ref="D51" r:id="rId53" xr:uid="{7A333D84-137A-4911-990B-4F0CD7B5700F}"/>
+    <hyperlink ref="D52" r:id="rId54" xr:uid="{87FA3EF4-9DD3-4F2E-8A17-D43CAC5E0FA8}"/>
+    <hyperlink ref="D53" r:id="rId55" xr:uid="{896679C3-0779-4141-990D-A15BB0BB031E}"/>
+    <hyperlink ref="D54" r:id="rId56" xr:uid="{87C6F2D0-3CFE-4C77-8960-A12C496D7394}"/>
+    <hyperlink ref="D55" r:id="rId57" xr:uid="{4B7EAE79-868F-4F85-8493-DB71E1B6717F}"/>
+    <hyperlink ref="F55" r:id="rId58" xr:uid="{ADE84154-F4EE-47E2-8A57-09BEC271F978}"/>
+    <hyperlink ref="D56" r:id="rId59" xr:uid="{655CC3F0-614B-49FE-B5E6-1F31A254E339}"/>
+    <hyperlink ref="F56" r:id="rId60" xr:uid="{CDBC077A-DC21-45C6-8AD0-DBCAF0E10694}"/>
+    <hyperlink ref="D57" r:id="rId61" xr:uid="{F1E167C4-5A5F-4850-A03D-95A6C29D87DE}"/>
+    <hyperlink ref="F57" r:id="rId62" xr:uid="{7198726F-1F14-40D2-A960-C7DF038D8639}"/>
+    <hyperlink ref="D58" r:id="rId63" xr:uid="{5C9E97E5-5EBB-4DFB-BE58-2AB3AE278691}"/>
+    <hyperlink ref="F58" r:id="rId64" xr:uid="{4A76750A-0F0E-407E-88C3-827C829CFA37}"/>
+    <hyperlink ref="D59" r:id="rId65" xr:uid="{B28EDBB0-C6CD-4B24-8866-3540EDD5E296}"/>
+    <hyperlink ref="F59" r:id="rId66" xr:uid="{5A888317-484D-4122-9A24-FF719129CBFD}"/>
+    <hyperlink ref="D60" r:id="rId67" xr:uid="{FB54205A-D412-4308-8365-4DE8596E8937}"/>
+    <hyperlink ref="F60" r:id="rId68" xr:uid="{4164942B-6DB2-4F66-B5D5-F8156ED4E2D6}"/>
+    <hyperlink ref="D61" r:id="rId69" xr:uid="{B2AE0F1A-BA42-4AD3-B285-F42B7259E4FC}"/>
+    <hyperlink ref="F61" r:id="rId70" xr:uid="{70791B82-23C0-4E3C-AE71-BB5C00A0BCEF}"/>
+    <hyperlink ref="D62" r:id="rId71" xr:uid="{5F0AD0C3-2BB4-4A86-A36C-6D17E4E5A416}"/>
+    <hyperlink ref="F62" r:id="rId72" xr:uid="{F66EB44A-1F4D-447B-B88A-8F7F073044C9}"/>
+    <hyperlink ref="D63" r:id="rId73" xr:uid="{975BFFC8-8079-4E3D-9898-AD9ECE38628D}"/>
+    <hyperlink ref="F63" r:id="rId74" xr:uid="{6B31BF36-66E5-4010-A807-AA456030E381}"/>
+    <hyperlink ref="D64" r:id="rId75" xr:uid="{CFC9CC61-2178-407C-B591-E1681E2D9C27}"/>
+    <hyperlink ref="F64" r:id="rId76" xr:uid="{67FEA0E6-7D97-4F24-9D0A-4E387E3747B2}"/>
+    <hyperlink ref="D65" r:id="rId77" xr:uid="{B462D26A-070A-4135-96F3-A86D241916C3}"/>
+    <hyperlink ref="F65" r:id="rId78" xr:uid="{C9DD4508-CD4F-4746-A4F6-83A49E4CFBF7}"/>
+    <hyperlink ref="D66" r:id="rId79" xr:uid="{32A7D8C7-5CAA-4B81-B8E7-CF7F7A8D8E6C}"/>
+    <hyperlink ref="F66" r:id="rId80" xr:uid="{07532909-CBB1-4D30-9C0A-FE67605D0605}"/>
+    <hyperlink ref="D67" r:id="rId81" xr:uid="{FB21B587-CA60-4C2D-81A3-0AE359871C78}"/>
+    <hyperlink ref="F67" r:id="rId82" xr:uid="{EC30A8A7-5182-4DE5-8221-A1E8FCEC713B}"/>
+    <hyperlink ref="D68" r:id="rId83" xr:uid="{777CB24E-7FFB-452E-BB52-1ACFA78CB26E}"/>
+    <hyperlink ref="F68" r:id="rId84" xr:uid="{A93F73B6-C5E7-4AF1-B24A-BB6752FC5841}"/>
+    <hyperlink ref="D69" r:id="rId85" xr:uid="{03754172-242E-40A5-B68C-4FC6DB94637B}"/>
+    <hyperlink ref="F69" r:id="rId86" xr:uid="{DFC43356-C64A-4287-8FFE-7E60A3044534}"/>
+    <hyperlink ref="D70" r:id="rId87" xr:uid="{35B221F8-8928-41DB-A384-FDC8663B5452}"/>
+    <hyperlink ref="F70" r:id="rId88" xr:uid="{623C58DD-ECBE-48B4-BD36-EDF8C1A92CEA}"/>
+    <hyperlink ref="D71" r:id="rId89" xr:uid="{F659BC3C-A08B-4A1A-ADB5-66B683DEF79C}"/>
+    <hyperlink ref="F71" r:id="rId90" xr:uid="{0B1D0A81-42CD-4D1B-A0A4-8AB7D4C63A71}"/>
+    <hyperlink ref="D72" r:id="rId91" xr:uid="{5806733E-1C3B-4C76-9E52-D9B7887C3B00}"/>
+    <hyperlink ref="F72" r:id="rId92" xr:uid="{47D336C5-00A8-4C81-884D-51186C757463}"/>
+    <hyperlink ref="D73" r:id="rId93" xr:uid="{8E65BFC0-3BE4-4AE2-96C6-E6348037316A}"/>
+    <hyperlink ref="F73" r:id="rId94" xr:uid="{B40FCA6C-EA63-4E1F-9BB6-7EF9590DB8E3}"/>
+    <hyperlink ref="D74" r:id="rId95" xr:uid="{D84B9B70-365D-4CDB-A314-F79A3CA4E77D}"/>
+    <hyperlink ref="F74" r:id="rId96" xr:uid="{80D8A644-70B5-4FDF-9BAD-39E0C8DB062A}"/>
+    <hyperlink ref="D75" r:id="rId97" xr:uid="{558E05B9-F85B-4477-BA67-CA43A8BA4B47}"/>
+    <hyperlink ref="F75" r:id="rId98" xr:uid="{23CA5105-449A-4E83-828B-1A1E18DE72C8}"/>
+    <hyperlink ref="D76" r:id="rId99" xr:uid="{CB378F21-32BD-4E04-8E7B-0FC693DA6144}"/>
+    <hyperlink ref="F76" r:id="rId100" xr:uid="{EAF9CC6D-8041-49A4-8072-99A78B35497F}"/>
+    <hyperlink ref="D77" r:id="rId101" xr:uid="{29256316-C74C-4AFC-BC63-48D31648C643}"/>
+    <hyperlink ref="F77" r:id="rId102" xr:uid="{22E5CC41-A064-4435-A9B1-4CACCBBC4A9C}"/>
+    <hyperlink ref="D78" r:id="rId103" xr:uid="{640EB0F0-ABEB-493A-BBA4-5D0F43ACB350}"/>
+    <hyperlink ref="F78" r:id="rId104" xr:uid="{94D73BE5-0DA0-4BCD-9532-493EB01A6CF8}"/>
+    <hyperlink ref="D79" r:id="rId105" xr:uid="{6ACC607E-4E7B-43E1-8F42-187761BD74A6}"/>
+    <hyperlink ref="F79" r:id="rId106" xr:uid="{EC4852F1-3AEC-44E9-B1B5-303B78ADBBA1}"/>
+    <hyperlink ref="D80" r:id="rId107" xr:uid="{969D087A-975C-4FED-8639-1D1644CAE54C}"/>
+    <hyperlink ref="F80" r:id="rId108" xr:uid="{0C0CDFF5-F423-4F73-A689-37CE315FBF4A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
busqueda New EP User
</commit_message>
<xml_diff>
--- a/Schuman List.xlsx
+++ b/Schuman List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\X1\Documents\Schuman\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14FA3522-72A2-4B3D-B30E-D221E4A0F046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E22DE50-91F2-41F0-97DD-6A628B80F411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{2FE17FE1-ABF7-4DC1-A8B0-257EE915A712}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="108">
   <si>
     <t>Agent</t>
   </si>
@@ -299,12 +299,12 @@
     <t>RITM0434593</t>
   </si>
   <si>
+    <t>Juan Carlos DIOSES</t>
+  </si>
+  <si>
     <t>Pending</t>
   </si>
   <si>
-    <t>Juan Carlos DIOSES</t>
-  </si>
-  <si>
     <t>SCTASK0887406</t>
   </si>
   <si>
@@ -320,159 +320,12 @@
     <t>SCTASK0880081</t>
   </si>
   <si>
-    <t>Natalia Maria VALENCIA AGUIRRE</t>
+    <t>Tania DE POORTER</t>
   </si>
   <si>
     <t>Complete</t>
   </si>
   <si>
-    <t>Georgiana SANDU</t>
-  </si>
-  <si>
-    <t>Klaudia ARBETOVA</t>
-  </si>
-  <si>
-    <t>Gabriel Stanislav Vladimir LITERA</t>
-  </si>
-  <si>
-    <t>Sandrina MARCUZZO</t>
-  </si>
-  <si>
-    <t>Marika SULANKO</t>
-  </si>
-  <si>
-    <t>Anastasia COUCOURATOS</t>
-  </si>
-  <si>
-    <t>Liselotte JENSEN</t>
-  </si>
-  <si>
-    <t>Lucie Agnès Marie Olga MAISTRELLI</t>
-  </si>
-  <si>
-    <t>Kristýna MAŤÁTKOVÁ</t>
-  </si>
-  <si>
-    <t>Ana RADOČAJ</t>
-  </si>
-  <si>
-    <t>Angelika KISS</t>
-  </si>
-  <si>
-    <t>Maria Nazareth ECHART ORUS</t>
-  </si>
-  <si>
-    <t>Krista DANKERE</t>
-  </si>
-  <si>
-    <t>Maja SABOL</t>
-  </si>
-  <si>
-    <t>Cristina SANCHEZ VILLA</t>
-  </si>
-  <si>
-    <t>Wojciech KUZMA</t>
-  </si>
-  <si>
-    <t>Tajana LJUBIČIĆ</t>
-  </si>
-  <si>
-    <t>Luc JEUNESSE</t>
-  </si>
-  <si>
-    <t>Maria Antoaneta NEAG</t>
-  </si>
-  <si>
-    <t>Kateřina HEROUTOVÁ</t>
-  </si>
-  <si>
-    <t>Igor DEQUECKER</t>
-  </si>
-  <si>
-    <t>Christos PAPAGIANNIS</t>
-  </si>
-  <si>
-    <t>Nicolas DORGERET</t>
-  </si>
-  <si>
-    <t>Ramune TAMASAUSKAITE</t>
-  </si>
-  <si>
-    <t>Cesar Augusto CASTELLO MORENO</t>
-  </si>
-  <si>
-    <t>Alina Leandra Ó RIADA</t>
-  </si>
-  <si>
-    <t>Francesco BARCHIELLI</t>
-  </si>
-  <si>
-    <t>Anna ARESU</t>
-  </si>
-  <si>
-    <t>Stephanie HONNEFELDER</t>
-  </si>
-  <si>
-    <t>Philine SCHOLZE</t>
-  </si>
-  <si>
-    <t>Ariane DEBYSER</t>
-  </si>
-  <si>
-    <t>Rachid AHAJJAM</t>
-  </si>
-  <si>
-    <t>Gianna GRIGÒ</t>
-  </si>
-  <si>
-    <t>Fabiola VALENTINI</t>
-  </si>
-  <si>
-    <t>Maria TOADER</t>
-  </si>
-  <si>
-    <t>Samuel DE LEMOS PEIXOTO</t>
-  </si>
-  <si>
-    <t>Elise HANCOTTE</t>
-  </si>
-  <si>
-    <t>Ellen Sarah VAN NIEUWENHUYZE</t>
-  </si>
-  <si>
-    <t>Anastasia MITRONATSIOU</t>
-  </si>
-  <si>
-    <t>5c7518931beb241018d65398624bcb08</t>
-  </si>
-  <si>
-    <t>David SCHWANDER</t>
-  </si>
-  <si>
-    <t>Karin SAUERTEIG</t>
-  </si>
-  <si>
-    <t>Barbara KRAFT</t>
-  </si>
-  <si>
-    <t>Virginie REMACLE</t>
-  </si>
-  <si>
-    <t>Ana SÁEZ-BENITO CAUVILLA</t>
-  </si>
-  <si>
-    <t>Bettina BLASIG</t>
-  </si>
-  <si>
-    <t>Cedric Franz K GOOR</t>
-  </si>
-  <si>
-    <t>Maria-teresa GONZALEZ CABALLERO</t>
-  </si>
-  <si>
-    <t>Tania DE POORTER</t>
-  </si>
-  <si>
     <t>Dora Cristina BARREIRA RAMOS</t>
   </si>
   <si>
@@ -507,9 +360,6 @@
   </si>
   <si>
     <t>Laura PROIETTI</t>
-  </si>
-  <si>
-    <t>New EP User</t>
   </si>
 </sst>
 </file>
@@ -913,7 +763,7 @@
   <dimension ref="A1:O80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B2:B9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -974,13 +824,13 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>89</v>
@@ -994,7 +844,7 @@
         <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>91</v>
@@ -1008,565 +858,265 @@
         <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
-        <v>94</v>
-      </c>
       <c r="D5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E5" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
-        <v>96</v>
-      </c>
       <c r="D6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E6" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B7" t="s">
-        <v>97</v>
-      </c>
       <c r="D7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E7" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
-        <v>98</v>
-      </c>
       <c r="D8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E8" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B9" t="s">
-        <v>99</v>
-      </c>
       <c r="D9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E9" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B10" t="s">
-        <v>100</v>
-      </c>
       <c r="D10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E10" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B11" t="s">
-        <v>101</v>
-      </c>
       <c r="D11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E11" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B12" t="s">
-        <v>102</v>
-      </c>
       <c r="D12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E12" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
-        <v>103</v>
-      </c>
       <c r="D13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E13" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
-        <v>104</v>
-      </c>
       <c r="D14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E14" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B15" t="s">
-        <v>105</v>
-      </c>
       <c r="D15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E15" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B16" t="s">
-        <v>106</v>
-      </c>
       <c r="D16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E16" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B17" t="s">
-        <v>107</v>
-      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D17" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E17" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B18" t="s">
-        <v>108</v>
-      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D18" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E18" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B19" t="s">
-        <v>109</v>
-      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D19" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E19" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B20" t="s">
-        <v>110</v>
-      </c>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D20" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E20" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B21" t="s">
-        <v>111</v>
-      </c>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D21" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E21" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B22" t="s">
-        <v>112</v>
-      </c>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D22" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E22" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B23" t="s">
-        <v>113</v>
-      </c>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D23" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E23" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B24" t="s">
-        <v>114</v>
-      </c>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D24" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E24" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B25" t="s">
-        <v>115</v>
-      </c>
+    </row>
+    <row r="25" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D25" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E25" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B26" t="s">
-        <v>116</v>
-      </c>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D26" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E26" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B27" t="s">
-        <v>117</v>
-      </c>
+    </row>
+    <row r="27" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D27" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E27" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B28" t="s">
-        <v>118</v>
-      </c>
+    </row>
+    <row r="28" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D28" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E28" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B29" t="s">
-        <v>119</v>
-      </c>
+    </row>
+    <row r="29" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D29" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E29" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B30" t="s">
-        <v>120</v>
-      </c>
+    </row>
+    <row r="30" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D30" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E30" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B31" t="s">
-        <v>121</v>
-      </c>
+    </row>
+    <row r="31" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D31" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E31" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B32" t="s">
-        <v>116</v>
-      </c>
+    </row>
+    <row r="32" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D32" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E32" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B33" t="s">
-        <v>122</v>
-      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D33" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E33" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B34" t="s">
-        <v>123</v>
-      </c>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D34" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E34" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B35" t="s">
-        <v>124</v>
-      </c>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D35" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E35" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B36" t="s">
-        <v>125</v>
-      </c>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D36" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E36" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B37" t="s">
-        <v>126</v>
-      </c>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D37" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E37" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B38" t="s">
-        <v>127</v>
-      </c>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D38" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E38" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B39" t="s">
-        <v>128</v>
-      </c>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D39" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E39" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B40" t="s">
-        <v>129</v>
-      </c>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D40" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E40" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B41" t="s">
-        <v>130</v>
-      </c>
+    </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D41" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E41" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B42" t="s">
-        <v>131</v>
-      </c>
+    </row>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D42" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E42" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B43" t="s">
-        <v>132</v>
-      </c>
+    </row>
+    <row r="43" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D43" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E43" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B44" t="s">
-        <v>133</v>
-      </c>
+    </row>
+    <row r="44" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D44" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E44" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B45" t="s">
-        <v>134</v>
-      </c>
+    </row>
+    <row r="45" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D45" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E45" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B46" t="s">
-        <v>135</v>
-      </c>
+    </row>
+    <row r="46" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D46" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E46" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B47" t="s">
-        <v>136</v>
-      </c>
+    </row>
+    <row r="47" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D47" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E47" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B48" t="s">
-        <v>137</v>
-      </c>
+    </row>
+    <row r="48" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D48" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E48" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B49" t="s">
-        <v>138</v>
-      </c>
       <c r="D49" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E49" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B50" t="s">
-        <v>139</v>
-      </c>
       <c r="D50" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E50" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B51" t="s">
-        <v>140</v>
-      </c>
       <c r="D51" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E51" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B52" t="s">
-        <v>141</v>
-      </c>
       <c r="D52" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E52" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B53" t="s">
-        <v>142</v>
-      </c>
       <c r="D53" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E53" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B54" t="s">
-        <v>143</v>
-      </c>
       <c r="D54" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E54" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B55" t="s">
-        <v>144</v>
+        <v>94</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>68</v>
@@ -1577,7 +1127,7 @@
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B56" t="s">
-        <v>144</v>
+        <v>94</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>68</v>
@@ -1588,7 +1138,7 @@
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B57" t="s">
-        <v>145</v>
+        <v>96</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>69</v>
@@ -1599,7 +1149,7 @@
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B58" t="s">
-        <v>145</v>
+        <v>96</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>69</v>
@@ -1610,7 +1160,7 @@
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B59" t="s">
-        <v>146</v>
+        <v>97</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>70</v>
@@ -1621,7 +1171,7 @@
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B60" t="s">
-        <v>146</v>
+        <v>97</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>70</v>
@@ -1632,7 +1182,7 @@
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B61" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>71</v>
@@ -1643,7 +1193,7 @@
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>71</v>
@@ -1654,7 +1204,7 @@
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B63" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>72</v>
@@ -1665,7 +1215,7 @@
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B64" t="s">
-        <v>147</v>
+        <v>98</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>73</v>
@@ -1676,7 +1226,7 @@
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B65" t="s">
-        <v>148</v>
+        <v>99</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>74</v>
@@ -1687,7 +1237,7 @@
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B66" t="s">
-        <v>149</v>
+        <v>100</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>75</v>
@@ -1698,7 +1248,7 @@
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B67" t="s">
-        <v>150</v>
+        <v>101</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>76</v>
@@ -1709,7 +1259,7 @@
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B68" t="s">
-        <v>151</v>
+        <v>102</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>77</v>
@@ -1720,7 +1270,7 @@
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B69" t="s">
-        <v>152</v>
+        <v>103</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>78</v>
@@ -1731,7 +1281,7 @@
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B70" t="s">
-        <v>153</v>
+        <v>104</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>79</v>
@@ -1742,7 +1292,7 @@
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B71" t="s">
-        <v>154</v>
+        <v>105</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>80</v>
@@ -1753,7 +1303,7 @@
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B72" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>81</v>
@@ -1764,7 +1314,7 @@
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B73" t="s">
-        <v>155</v>
+        <v>106</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>82</v>
@@ -1775,7 +1325,7 @@
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B74" t="s">
-        <v>156</v>
+        <v>107</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>83</v>
@@ -1786,7 +1336,7 @@
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B75" t="s">
-        <v>156</v>
+        <v>107</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>83</v>
@@ -1797,29 +1347,29 @@
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B76" t="s">
-        <v>157</v>
+        <v>87</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>84</v>
       </c>
       <c r="E76" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B77" t="s">
-        <v>157</v>
+        <v>87</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>84</v>
       </c>
       <c r="E77" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B78" t="s">
-        <v>157</v>
+        <v>87</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>85</v>
@@ -1830,7 +1380,7 @@
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B79" t="s">
-        <v>157</v>
+        <v>87</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>86</v>
@@ -1841,7 +1391,7 @@
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B80" t="s">
-        <v>157</v>
+        <v>87</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>86</v>

</xml_diff>

<commit_message>
Add a new graphical user interface for the Schuman Word Generator.
</commit_message>
<xml_diff>
--- a/Schuman List.xlsx
+++ b/Schuman List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\X1\Documents\Schuman\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6DE5E1-C49E-4573-8D34-2B6BA81F5831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D691B3-B9C9-4C78-BB37-A363B4DD5631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{2FE17FE1-ABF7-4DC1-A8B0-257EE915A712}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="35">
   <si>
     <t>Agent</t>
   </si>
@@ -135,6 +135,12 @@
   </si>
   <si>
     <t>SCTASK0765919</t>
+  </si>
+  <si>
+    <t>MUSTBRUN2425474</t>
+  </si>
+  <si>
+    <t>MUSTBRUN2423960</t>
   </si>
 </sst>
 </file>
@@ -631,6 +637,9 @@
       <c r="B4" t="s">
         <v>28</v>
       </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
       <c r="D4" s="3" t="s">
         <v>17</v>
       </c>
@@ -642,6 +651,9 @@
       <c r="B5" t="s">
         <v>28</v>
       </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
       <c r="D5" s="3" t="s">
         <v>17</v>
       </c>
@@ -664,6 +676,9 @@
       <c r="B7" t="s">
         <v>31</v>
       </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
       <c r="D7" s="3" t="s">
         <v>19</v>
       </c>
@@ -674,6 +689,9 @@
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
check int the issue with check in and out
</commit_message>
<xml_diff>
--- a/Schuman List.xlsx
+++ b/Schuman List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\X1\Documents\Schuman\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DCFB9AB-FB6B-4651-B584-A61EB84B219B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CAA654B-42C6-4B4A-83F5-B1458AA9509E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2660" yWindow="2660" windowWidth="14400" windowHeight="8170" xr2:uid="{2FE17FE1-ABF7-4DC1-A8B0-257EE915A712}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11175" xr2:uid="{2FE17FE1-ABF7-4DC1-A8B0-257EE915A712}"/>
   </bookViews>
   <sheets>
     <sheet name="BRU" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>Agent</t>
   </si>
@@ -98,73 +98,40 @@
     <t>RITM0420972</t>
   </si>
   <si>
-    <t>RITM0434588</t>
-  </si>
-  <si>
-    <t>RITM0434592</t>
-  </si>
-  <si>
     <t>RITM0434593</t>
   </si>
   <si>
     <t>Juan Carlos DIOSES</t>
   </si>
   <si>
+    <t>MUSTBRUN2424012</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>Alexandra DE TORNACO</t>
+  </si>
+  <si>
     <t>Pending</t>
   </si>
   <si>
+    <t>SCTASK0784120, SCTASK0784119</t>
+  </si>
+  <si>
+    <t>Devrim ATES</t>
+  </si>
+  <si>
+    <t>Jauram REISNER</t>
+  </si>
+  <si>
+    <t>Laura PROIETTI</t>
+  </si>
+  <si>
+    <t>Checked-Out</t>
+  </si>
+  <si>
     <t>SCTASK0887406</t>
-  </si>
-  <si>
-    <t>SCTASK0784120, SCTASK0784119</t>
-  </si>
-  <si>
-    <t>Devrim ATES</t>
-  </si>
-  <si>
-    <t>Complete</t>
-  </si>
-  <si>
-    <t>SCTASK0765919</t>
-  </si>
-  <si>
-    <t>MUSTBRUN2425474</t>
-  </si>
-  <si>
-    <t>Alexandra DE TORNACO</t>
-  </si>
-  <si>
-    <t>Jauram REISNER</t>
-  </si>
-  <si>
-    <t>Laura PROIETTI</t>
-  </si>
-  <si>
-    <t>OK</t>
-  </si>
-  <si>
-    <t>C:\Users\X1\Documents\Schuman\WORD files\RITM0496748_Juan Carlos DIOSES (2).pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\X1\Documents\Schuman\WORD files\RITM0405052_Alexandra DE TORNACO.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\X1\Documents\Schuman\WORD files\RITM0400334_Devrim ATES.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\X1\Documents\Schuman\WORD files\RITM0433331_Jauram REISNER.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\X1\Documents\Schuman\WORD files\RITM0420972_Laura PROIETTI.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\X1\Documents\Schuman\WORD files\RITM0434588_Juan Carlos DIOSES.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\X1\Documents\Schuman\WORD files\RITM0434592_Juan Carlos DIOSES.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\X1\Documents\Schuman\WORD files\RITM0434593_Juan Carlos DIOSES.pdf</t>
   </si>
 </sst>
 </file>
@@ -222,13 +189,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -565,24 +533,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D15FE3B-AD84-45CF-9592-EB018CC38643}">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" workbookViewId="0">
-      <selection activeCell="C15" sqref="A6:C15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="38.453125" customWidth="1"/>
-    <col min="3" max="3" width="29.7265625" customWidth="1"/>
+    <col min="2" max="2" width="38.42578125" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="18.08984375" customWidth="1"/>
-    <col min="6" max="6" width="14.90625" customWidth="1"/>
-    <col min="11" max="11" width="29.453125" customWidth="1"/>
-    <col min="14" max="14" width="37.1796875" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" customWidth="1"/>
+    <col min="11" max="11" width="29.42578125" customWidth="1"/>
+    <col min="14" max="14" width="37.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -629,242 +597,95 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>23</v>
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="4">
+        <v>46076.395428240743</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>24</v>
-      </c>
-      <c r="F2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" t="s">
-        <v>34</v>
-      </c>
-      <c r="J2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
-        <v>31</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
         <v>26</v>
       </c>
-      <c r="H3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" t="s">
-        <v>36</v>
-      </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>27</v>
       </c>
-      <c r="C4" t="s">
-        <v>30</v>
-      </c>
       <c r="D4" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>28</v>
       </c>
-      <c r="H4" t="s">
-        <v>34</v>
-      </c>
-      <c r="J4" t="s">
-        <v>37</v>
+      <c r="D5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" t="s">
-        <v>34</v>
-      </c>
-      <c r="J5" t="s">
-        <v>37</v>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" t="s">
-        <v>34</v>
-      </c>
-      <c r="J7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" t="s">
-        <v>34</v>
-      </c>
-      <c r="J8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B9" t="s">
         <v>23</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H9" t="s">
-        <v>34</v>
-      </c>
-      <c r="J9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" t="s">
-        <v>29</v>
-      </c>
-      <c r="H10" t="s">
-        <v>34</v>
-      </c>
-      <c r="J10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" t="s">
-        <v>28</v>
-      </c>
-      <c r="H11" t="s">
-        <v>34</v>
-      </c>
-      <c r="J11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" t="s">
-        <v>28</v>
-      </c>
-      <c r="H12" t="s">
-        <v>34</v>
-      </c>
-      <c r="J12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" t="s">
-        <v>28</v>
-      </c>
-      <c r="H13" t="s">
-        <v>34</v>
-      </c>
-      <c r="J13" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{BA17A53B-7B69-4A8F-B5D5-943D15D604FE}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{9990B10D-1867-43D9-BA0D-47C428B6CBCD}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{B28EDBB0-C6CD-4B24-8866-3540EDD5E296}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{FB54205A-D412-4308-8365-4DE8596E8937}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{8E65BFC0-3BE4-4AE2-96C6-E6348037316A}"/>
-    <hyperlink ref="D7" r:id="rId6" xr:uid="{D84B9B70-365D-4CDB-A314-F79A3CA4E77D}"/>
-    <hyperlink ref="D8" r:id="rId7" xr:uid="{558E05B9-F85B-4477-BA67-CA43A8BA4B47}"/>
-    <hyperlink ref="D9" r:id="rId8" xr:uid="{CB378F21-32BD-4E04-8E7B-0FC693DA6144}"/>
-    <hyperlink ref="D10" r:id="rId9" xr:uid="{29256316-C74C-4AFC-BC63-48D31648C643}"/>
-    <hyperlink ref="D11" r:id="rId10" xr:uid="{640EB0F0-ABEB-493A-BBA4-5D0F43ACB350}"/>
-    <hyperlink ref="D12" r:id="rId11" xr:uid="{6ACC607E-4E7B-43E1-8F42-187761BD74A6}"/>
-    <hyperlink ref="D13" r:id="rId12" xr:uid="{969D087A-975C-4FED-8639-1D1644CAE54C}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{FB54205A-D412-4308-8365-4DE8596E8937}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{8E65BFC0-3BE4-4AE2-96C6-E6348037316A}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{558E05B9-F85B-4477-BA67-CA43A8BA4B47}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{969D087A-975C-4FED-8639-1D1644CAE54C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>